<commit_message>
cleaned files and added button
added button to download daily data Excel
</commit_message>
<xml_diff>
--- a/output/partners_district_data.xlsx
+++ b/output/partners_district_data.xlsx
@@ -3424,7 +3424,7 @@
         <v>137</v>
       </c>
       <c r="E53" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F53"/>
       <c r="G53"/>
@@ -5206,7 +5206,7 @@
         <v>228</v>
       </c>
       <c r="E101" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F101"/>
       <c r="G101"/>
@@ -5455,7 +5455,7 @@
         <v>242</v>
       </c>
       <c r="E108" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F108"/>
       <c r="G108"/>
@@ -5962,7 +5962,7 @@
         <v>270</v>
       </c>
       <c r="E121" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F121"/>
       <c r="G121"/>
@@ -5999,7 +5999,7 @@
         <v>272</v>
       </c>
       <c r="E122" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F122"/>
       <c r="G122"/>

</xml_diff>